<commit_message>
Common: Preparing cell stuff
</commit_message>
<xml_diff>
--- a/fixtures/cells.xlsx
+++ b/fixtures/cells.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEBEBB1-50B4-4F8F-BC83-6231207629DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7274D9B6-540E-4581-BE08-0A873D069024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="2625" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="1725" windowWidth="23610" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>tab</t>
   </si>
@@ -52,15 +52,9 @@
     <t>HG2</t>
   </si>
   <si>
-    <t>3.7</t>
-  </si>
-  <si>
     <t>cells</t>
   </si>
   <si>
-    <t>PuffSmith\Cell\Import\CellImport</t>
-  </si>
-  <si>
     <t>Sony</t>
   </si>
   <si>
@@ -77,6 +71,15 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>cell</t>
+  </si>
+  <si>
+    <t>KeepPower</t>
+  </si>
+  <si>
+    <t>IMR18350</t>
   </si>
 </sst>
 </file>
@@ -131,11 +134,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -440,10 +445,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -453,10 +458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D14216-B959-4E8A-B472-89E49CBB65F3}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +470,7 @@
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -481,8 +486,8 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -492,69 +497,86 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
+      <c r="C2" s="4">
+        <v>3.7</v>
       </c>
       <c r="D2">
         <v>20</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>18650</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3.7</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>18650</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
+      <c r="C4" s="4">
+        <v>3.7</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>18650</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.7</v>
       </c>
       <c r="D5">
         <v>35</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>21700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="6">
+        <v>18350</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>